<commit_message>
Mudanças no valor da colher de sopa da aveia, e inclusão da pesquisa no select
</commit_message>
<xml_diff>
--- a/MedidasIngredientes.xlsx
+++ b/MedidasIngredientes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
   <si>
     <t>Açucar</t>
   </si>
@@ -250,6 +250,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,16 +276,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -570,7 +570,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,39 +586,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -644,43 +644,43 @@
       <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
+      <c r="H3" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="6">
         <v>144</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="6">
         <v>9</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="12">
+      <c r="F5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="6">
         <v>3</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -695,703 +695,714 @@
       <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6">
         <v>128</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="6">
         <v>8</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="6">
         <v>6</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="6">
         <v>3</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="6">
         <v>150</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="6">
         <v>185</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="D9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6">
         <v>12</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="6">
         <v>8</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="6">
         <v>4</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="12">
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6">
         <v>80</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="D11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6">
         <v>5</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="12">
+      <c r="G11" s="6">
         <v>1.5</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="6">
         <v>170</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="6">
         <v>200</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="6">
         <v>220</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="6">
         <v>14</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="6">
         <v>9</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="6">
         <v>4.5</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="6">
         <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="6">
         <v>184</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="6">
         <v>224</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="D15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="6">
         <v>14</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="6">
         <v>10</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="6">
         <v>5</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="6">
         <v>66</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="6">
         <v>80</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="D17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="6">
         <v>5</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="6">
         <v>4</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="6">
         <v>2</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="6">
         <v>5</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="12">
+      <c r="F19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="6">
         <v>1.5</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="6">
         <v>115</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="6">
         <v>140</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="6">
         <v>9</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="6">
         <v>6</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="6">
         <v>3</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="6">
         <v>74</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="6">
         <v>90</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="12">
+      <c r="D23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="6">
         <v>6</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="6">
         <v>4</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="6">
         <v>2</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="6">
         <v>100</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="6">
         <v>7</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="6">
         <v>2</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="H25" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="5"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="12">
+      <c r="B27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="6">
         <v>80</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="12">
+      <c r="D27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="6">
         <v>5</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="12">
+      <c r="F27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="6">
         <v>1.5</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="5"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="12">
+      <c r="B29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="6">
         <v>150</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="12">
+      <c r="D29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="6">
         <v>9</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29" s="12">
+      <c r="F29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="6">
         <v>3</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="5"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="6">
         <v>165</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="6">
         <v>165</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="6">
         <v>212</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="6">
         <v>13</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="6">
         <v>5</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="6">
         <v>2</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="5"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="12">
+      <c r="B33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="6">
         <v>230</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="12">
+      <c r="D33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="6">
         <v>30</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G33" s="12">
+      <c r="F33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="6">
         <v>10</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="5"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="6">
         <v>104</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="6">
         <v>126</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="12">
+      <c r="D37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="6">
         <v>7.9</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="6">
         <v>5.25</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="6">
         <v>2.6</v>
       </c>
-      <c r="H37" s="12" t="s">
+      <c r="H37" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="6">
         <v>165</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="6">
         <v>200</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="12">
+      <c r="D39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="6">
         <v>12.5</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39" s="6">
         <v>8.4</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="6">
         <v>4.2</v>
       </c>
-      <c r="H39" s="12" t="s">
+      <c r="H39" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="5"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="6">
         <v>246</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="6">
         <v>300</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E41" s="12">
+      <c r="D41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="6">
         <v>18</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41" s="6">
         <v>12</v>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="6">
         <v>6</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="5"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="6">
         <v>105</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="6">
         <v>128</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="12">
+      <c r="D43" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="6">
         <v>8</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="6">
         <v>5.2</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="6">
         <v>2.6</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="H43" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="5"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="6">
         <v>200</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45" s="6">
         <v>150</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45" s="6">
         <v>250</v>
       </c>
-      <c r="E45" s="12">
+      <c r="E45" s="6">
         <v>15</v>
       </c>
-      <c r="F45" s="12">
+      <c r="F45" s="6">
         <v>10</v>
       </c>
-      <c r="G45" s="12">
+      <c r="G45" s="6">
         <v>5</v>
       </c>
-      <c r="H45" s="12">
+      <c r="H45" s="6">
         <v>2.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="A42:H42"/>
@@ -1402,18 +1413,7 @@
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A26:H26"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>